<commit_message>
CIERRE 24 MAY 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ASIGNACIONES  VEHICULOS   2021.xlsx
+++ b/01 DOCUEMENTOS/ASIGNACIONES  VEHICULOS   2021.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01 DOCUEMENTOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E8E8C7-02A8-4893-8470-A2CA4E6D5722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="1545" windowWidth="15900" windowHeight="13650" xr2:uid="{9BC95958-1897-4B40-A26F-D1112CF8CD60}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17670" windowHeight="11220"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -363,7 +362,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,7 +415,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -437,6 +436,12 @@
     <fill>
       <patternFill patternType="darkVertical"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -593,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -608,9 +613,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -709,11 +711,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,21 +1148,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059F58DF-0966-474A-A73C-7FF8517E9DF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="39" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="34" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="34"/>
-    <col min="4" max="4" width="15.85546875" style="35" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="34" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="36" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="38" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="33" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="33"/>
+    <col min="4" max="4" width="15.85546875" style="34" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="33" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1165,27 +1173,27 @@
       <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="31" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1197,7 +1205,7 @@
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1205,7 +1213,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1217,7 +1225,7 @@
       <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1225,7 +1233,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1237,7 +1245,7 @@
       <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1245,7 +1253,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1257,7 +1265,7 @@
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1265,7 +1273,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1277,7 +1285,7 @@
       <c r="D7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="24" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1285,7 +1293,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1294,10 +1302,10 @@
       <c r="C8" s="5">
         <v>2015</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="25" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1305,7 +1313,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="16">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1317,7 +1325,7 @@
       <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -1325,7 +1333,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="A10" s="16">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1337,7 +1345,7 @@
       <c r="D10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="26" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1345,7 +1353,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="A11" s="16">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1354,10 +1362,10 @@
       <c r="C11" s="5">
         <v>2015</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="26" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1365,7 +1373,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="A12" s="16">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1377,7 +1385,7 @@
       <c r="D12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="26" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1385,7 +1393,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
+      <c r="A13" s="16">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1397,7 +1405,7 @@
       <c r="D13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -1405,7 +1413,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
+      <c r="A14" s="16">
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1417,7 +1425,7 @@
       <c r="D14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -1425,7 +1433,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+      <c r="A15" s="16">
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1437,7 +1445,7 @@
       <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="24" t="s">
         <v>34</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -1445,7 +1453,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
+      <c r="A16" s="16">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1457,7 +1465,7 @@
       <c r="D16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>37</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -1465,7 +1473,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
+      <c r="A17" s="16">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1477,7 +1485,7 @@
       <c r="D17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -1485,7 +1493,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="A18" s="16">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1497,7 +1505,7 @@
       <c r="D18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="26" t="s">
         <v>43</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -1505,7 +1513,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+      <c r="A19" s="16">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1517,15 +1525,15 @@
       <c r="D19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="26" t="s">
         <v>46</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
+    <row r="20" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1537,15 +1545,15 @@
       <c r="D20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>49</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
+    <row r="21" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1557,188 +1565,188 @@
       <c r="D21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="27" t="s">
         <v>51</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+    <row r="22" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
         <v>20</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>2021</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>54</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+    <row r="23" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>2021</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="27" t="s">
         <v>56</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+    <row r="24" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
         <v>22</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>2018</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="27" t="s">
         <v>58</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="7" t="s">
+    <row r="25" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>2021</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="29" t="s">
         <v>61</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="7" t="s">
+    <row r="27" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>2012</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="30" t="s">
         <v>64</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="7" t="s">
+    <row r="28" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>2010</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="27" t="s">
         <v>67</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
+    <row r="29" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
         <v>24</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>2012</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="27" t="s">
         <v>70</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21">
+    <row r="31" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20">
         <v>26</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>2020</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="26" t="s">
         <v>73</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="21">
+    <row r="32" spans="1:6" s="40" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="20">
         <v>28</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C32" s="2">
@@ -1747,46 +1755,46 @@
       <c r="D32" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="24" t="s">
         <v>76</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="13" t="s">
+    <row r="33" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
+      <c r="B33" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="40">
+      <c r="C33" s="39">
         <v>2019</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="42" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-      <c r="B34" s="7" t="s">
+    <row r="34" spans="1:6" s="40" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="36"/>
+      <c r="B34" s="6" t="s">
         <v>80</v>
       </c>
       <c r="C34" s="2">
         <v>2019</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="38"/>
+      <c r="F34" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>